<commit_message>
Fix: Updated config and changes bool for sending email. sends email if false.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="0" windowWidth="21255" windowHeight="8070" activeTab="2"/>
+    <workbookView xWindow="-10245" yWindow="0" windowWidth="21255" windowHeight="8070"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -44,9 +44,6 @@
     <t>ExScreenshotsFolderPath</t>
   </si>
   <si>
-    <t>Exceptions_Screenshots</t>
-  </si>
-  <si>
     <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -185,9 +179,6 @@
     <t>Cred_NA_OeP</t>
   </si>
   <si>
-    <t>OrchestratorQueueNameSammanstallning</t>
-  </si>
-  <si>
     <t>MergeFilePath</t>
   </si>
   <si>
@@ -216,13 +207,52 @@
   </si>
   <si>
     <t>FolderPathToManagedFiles</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>\\safs008\RPA\VoF\RPA_030\Temp</t>
+  </si>
+  <si>
+    <t>Sammanställning av PDF</t>
+  </si>
+  <si>
+    <t>ProcessingPrefix</t>
+  </si>
+  <si>
+    <t>_Hanteras</t>
+  </si>
+  <si>
+    <t>FinishedPrefix</t>
+  </si>
+  <si>
+    <t>_Klar</t>
+  </si>
+  <si>
+    <t>mailrelay.sundsvall.se</t>
+  </si>
+  <si>
+    <t>RPA-no-reply@sundsvall.se</t>
+  </si>
+  <si>
+    <t>http://www.oeplatform.org/version/2.0/schemas/flowinstance</t>
+  </si>
+  <si>
+    <t>PDFSammanställning</t>
+  </si>
+  <si>
+    <t>FinishedCaseStatus</t>
+  </si>
+  <si>
+    <t>Klart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -246,6 +276,30 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -267,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -277,6 +331,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,14 +654,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="59.28515625" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -641,49 +702,100 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1680,7 +1792,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1733,29 +1845,29 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1764,112 +1876,112 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="45">
       <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B18" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2851,9 +2963,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2873,7 +2985,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2903,127 +3015,92 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>55</v>
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -4003,11 +4080,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>